<commit_message>
modified:   CMF-MySQL_Azure_SingleServer_to_Flexible.ps1 	modified:   CMF-MySQL_Single_Server_Input_file.xlsx
</commit_message>
<xml_diff>
--- a/CMF-MySQL_Single_Server_Input_file.xlsx
+++ b/CMF-MySQL_Single_Server_Input_file.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-madagrawal\Desktop\Microsoft\mysql_flexible\Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D597D54-9D7D-49BD-8660-AC4EE521E9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9FE6A2-9C22-4BF3-9955-FD79F47CE024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Azure_Subscription" sheetId="2" r:id="rId1"/>
     <sheet name="Server_List" sheetId="3" r:id="rId2"/>
+    <sheet name="Reference" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Server_List!$A$1:$P$3</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="89">
   <si>
     <t>Host_Name</t>
   </si>
@@ -123,17 +127,194 @@
     <t>NO</t>
   </si>
   <si>
-    <t>promysqlflexibleSSL3</t>
-  </si>
-  <si>
-    <t>promysqlflexible</t>
+    <t>Burstable</t>
+  </si>
+  <si>
+    <t>promysqlFlexible1</t>
+  </si>
+  <si>
+    <t>Standard_B1ms</t>
+  </si>
+  <si>
+    <t>Compute size</t>
+  </si>
+  <si>
+    <t>vCores</t>
+  </si>
+  <si>
+    <t>Memory Size (GiB)</t>
+  </si>
+  <si>
+    <t>Max Supported IOPS</t>
+  </si>
+  <si>
+    <t>Max Connections</t>
+  </si>
+  <si>
+    <t>Temp Storage (SSD) GiB</t>
+  </si>
+  <si>
+    <t>Standard_B1s</t>
+  </si>
+  <si>
+    <t>Standard_B2s</t>
+  </si>
+  <si>
+    <t>Standard_B2ms</t>
+  </si>
+  <si>
+    <t>Standard_B4ms</t>
+  </si>
+  <si>
+    <t>Standard_B8ms</t>
+  </si>
+  <si>
+    <t>Standard_B12ms</t>
+  </si>
+  <si>
+    <t>Standard_B16ms</t>
+  </si>
+  <si>
+    <t>Standard_B20ms</t>
+  </si>
+  <si>
+    <t>Standard_D2ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_D4ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_D4ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_D8ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_D8ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_D16ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_D16ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_D32ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_D32ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_D48ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_D48ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_D64ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_D64ds_v4</t>
+  </si>
+  <si>
+    <t>Business Critical</t>
+  </si>
+  <si>
+    <t>Standard_E2ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_E2ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_E4ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_E4ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_E8ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_E8ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_E16ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_E16ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_E20ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_E20ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_E32ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_E32ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_E48ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_E48ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_E64ds_v4</t>
+  </si>
+  <si>
+    <t>Standard_E64ads_v5</t>
+  </si>
+  <si>
+    <t>Standard_E80ids_v4</t>
+  </si>
+  <si>
+    <t>Standard_E2ds_v5</t>
+  </si>
+  <si>
+    <t>Standard_E4ds_v5</t>
+  </si>
+  <si>
+    <t>Standard_E8ds_v5</t>
+  </si>
+  <si>
+    <t>Standard_E16ds_v5</t>
+  </si>
+  <si>
+    <t>Standard_E20ds_v5</t>
+  </si>
+  <si>
+    <t>Standard_E32ds_v5</t>
+  </si>
+  <si>
+    <t>Standard_E48ds_v5</t>
+  </si>
+  <si>
+    <t>Standard_E64ds_v5</t>
+  </si>
+  <si>
+    <t>Standard_E96ds_v5</t>
+  </si>
+  <si>
+    <t>General Purpose</t>
+  </si>
+  <si>
+    <t>MemoryOptimized</t>
+  </si>
+  <si>
+    <t>promysqlFlexible2</t>
+  </si>
+  <si>
+    <t>promysqlsingle1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +346,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF8B0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF292827"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF161616"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF161616"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF161616"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +388,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -207,12 +425,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A26AFE-32F2-4493-A9DC-655EA3B3D244}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="78" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,8 +777,8 @@
     <col min="9" max="9" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.90625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.90625" bestFit="1" customWidth="1"/>
@@ -589,10 +819,10 @@
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>21</v>
@@ -629,16 +859,16 @@
         <v>10</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>18</v>
+      <c r="L2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="N2" s="3">
         <v>20</v>
@@ -670,26 +900,1420 @@
       <c r="I3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="L3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" s="3">
+        <v>20</v>
+      </c>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K3" xr:uid="{8C5F2BF3-BAAC-4979-937C-9A68EF8F0646}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K4" xr:uid="{8C5F2BF3-BAAC-4979-937C-9A68EF8F0646}">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{5FB8D6A8-F1C2-4D6C-A640-9755E22E8A11}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2 N4" xr:uid="{5FB8D6A8-F1C2-4D6C-A640-9755E22E8A11}">
       <formula1>20</formula1>
       <formula2>16000</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L4" xr:uid="{645C3E52-F12F-4B72-8D7E-2B12914E6CD3}">
+      <formula1>"Burstable,GeneralPurpose,MemoryOptimized"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{E3BEC63F-02FB-47DF-AC86-27B190EC0389}">
+      <formula1>3</formula1>
+      <formula2>63</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error" error="Incorrect value entered" promptTitle="Sku-Name" prompt="Please refer Reference sheet for valid input." xr:uid="{AFF2D7CA-0596-4B9F-B46C-96AB2EB94A31}">
+          <x14:formula1>
+            <xm:f>IF($L2="Burstable",Reference!$C$2:$C$10,IF($L2="GeneralPurpose",Reference!$C$11:$C$24,IF($L2="MemoryOptimized",Reference!$C$25:$C$50)))</xm:f>
+          </x14:formula1>
+          <xm:sqref>M2:M4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A58AE5-72CE-4DB2-93BD-67BB82644CC0}">
+  <dimension ref="A1:H50"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8">
+        <v>320</v>
+      </c>
+      <c r="G2" s="8">
+        <v>171</v>
+      </c>
+      <c r="H2" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2</v>
+      </c>
+      <c r="F3" s="8">
+        <v>640</v>
+      </c>
+      <c r="G3" s="8">
+        <v>341</v>
+      </c>
+      <c r="H3" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1280</v>
+      </c>
+      <c r="G4" s="8">
+        <v>683</v>
+      </c>
+      <c r="H4" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1700</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1365</v>
+      </c>
+      <c r="H5" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="8">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2400</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2731</v>
+      </c>
+      <c r="H6" s="8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="8">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8">
+        <v>32</v>
+      </c>
+      <c r="F7" s="8">
+        <v>3100</v>
+      </c>
+      <c r="G7" s="8">
+        <v>5461</v>
+      </c>
+      <c r="H7" s="8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="8">
+        <v>12</v>
+      </c>
+      <c r="E8" s="8">
+        <v>48</v>
+      </c>
+      <c r="F8" s="8">
+        <v>3800</v>
+      </c>
+      <c r="G8" s="8">
+        <v>8193</v>
+      </c>
+      <c r="H8" s="8">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="8">
+        <v>16</v>
+      </c>
+      <c r="E9" s="8">
+        <v>64</v>
+      </c>
+      <c r="F9" s="8">
+        <v>4300</v>
+      </c>
+      <c r="G9" s="8">
+        <v>10923</v>
+      </c>
+      <c r="H9" s="8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="8">
+        <v>20</v>
+      </c>
+      <c r="E10" s="8">
+        <v>80</v>
+      </c>
+      <c r="F10" s="8">
+        <v>5000</v>
+      </c>
+      <c r="G10" s="8">
+        <v>13653</v>
+      </c>
+      <c r="H10" s="8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>8</v>
+      </c>
+      <c r="F11" s="8">
+        <v>3200</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1365</v>
+      </c>
+      <c r="H11" s="8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="8">
+        <v>2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>8</v>
+      </c>
+      <c r="F12" s="8">
+        <v>3200</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1365</v>
+      </c>
+      <c r="H12" s="8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="8">
+        <v>4</v>
+      </c>
+      <c r="E13" s="8">
+        <v>16</v>
+      </c>
+      <c r="F13" s="8">
+        <v>6400</v>
+      </c>
+      <c r="G13" s="8">
+        <v>2731</v>
+      </c>
+      <c r="H13" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="8">
+        <v>4</v>
+      </c>
+      <c r="E14" s="8">
+        <v>16</v>
+      </c>
+      <c r="F14" s="8">
+        <v>6400</v>
+      </c>
+      <c r="G14" s="8">
+        <v>2731</v>
+      </c>
+      <c r="H14" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="8">
+        <v>8</v>
+      </c>
+      <c r="E15" s="8">
+        <v>32</v>
+      </c>
+      <c r="F15" s="8">
+        <v>12800</v>
+      </c>
+      <c r="G15" s="8">
+        <v>5461</v>
+      </c>
+      <c r="H15" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="8">
+        <v>8</v>
+      </c>
+      <c r="E16" s="8">
+        <v>32</v>
+      </c>
+      <c r="F16" s="8">
+        <v>12800</v>
+      </c>
+      <c r="G16" s="8">
+        <v>5461</v>
+      </c>
+      <c r="H16" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="8">
+        <v>16</v>
+      </c>
+      <c r="E17" s="8">
+        <v>64</v>
+      </c>
+      <c r="F17" s="8">
+        <v>20000</v>
+      </c>
+      <c r="G17" s="8">
+        <v>10923</v>
+      </c>
+      <c r="H17" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="8">
+        <v>16</v>
+      </c>
+      <c r="E18" s="8">
+        <v>64</v>
+      </c>
+      <c r="F18" s="8">
+        <v>20000</v>
+      </c>
+      <c r="G18" s="8">
+        <v>10923</v>
+      </c>
+      <c r="H18" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="8">
+        <v>32</v>
+      </c>
+      <c r="E19" s="8">
+        <v>128</v>
+      </c>
+      <c r="F19" s="8">
+        <v>20000</v>
+      </c>
+      <c r="G19" s="8">
+        <v>21845</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="8">
+        <v>32</v>
+      </c>
+      <c r="E20" s="8">
+        <v>128</v>
+      </c>
+      <c r="F20" s="8">
+        <v>20000</v>
+      </c>
+      <c r="G20" s="8">
+        <v>21845</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="8">
+        <v>48</v>
+      </c>
+      <c r="E21" s="8">
+        <v>192</v>
+      </c>
+      <c r="F21" s="8">
+        <v>20000</v>
+      </c>
+      <c r="G21" s="8">
+        <v>32768</v>
+      </c>
+      <c r="H21" s="8">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="8">
+        <v>48</v>
+      </c>
+      <c r="E22" s="8">
+        <v>192</v>
+      </c>
+      <c r="F22" s="8">
+        <v>20000</v>
+      </c>
+      <c r="G22" s="8">
+        <v>32768</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="8">
+        <v>64</v>
+      </c>
+      <c r="E23" s="8">
+        <v>256</v>
+      </c>
+      <c r="F23" s="8">
+        <v>20000</v>
+      </c>
+      <c r="G23" s="8">
+        <v>43691</v>
+      </c>
+      <c r="H23" s="8">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="8">
+        <v>64</v>
+      </c>
+      <c r="E24" s="8">
+        <v>256</v>
+      </c>
+      <c r="F24" s="8">
+        <v>20000</v>
+      </c>
+      <c r="G24" s="8">
+        <v>43691</v>
+      </c>
+      <c r="H24" s="8">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="8">
+        <v>2</v>
+      </c>
+      <c r="E25" s="8">
+        <v>16</v>
+      </c>
+      <c r="F25" s="8">
+        <v>5000</v>
+      </c>
+      <c r="G25" s="8">
+        <v>2731</v>
+      </c>
+      <c r="H25" s="8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="8">
+        <v>2</v>
+      </c>
+      <c r="E26" s="8">
+        <v>16</v>
+      </c>
+      <c r="F26" s="8">
+        <v>5000</v>
+      </c>
+      <c r="G26" s="8">
+        <v>2731</v>
+      </c>
+      <c r="H26" s="8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="8">
+        <v>4</v>
+      </c>
+      <c r="E27" s="8">
+        <v>32</v>
+      </c>
+      <c r="F27" s="8">
+        <v>10000</v>
+      </c>
+      <c r="G27" s="8">
+        <v>5461</v>
+      </c>
+      <c r="H27" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="8">
+        <v>4</v>
+      </c>
+      <c r="E28" s="8">
+        <v>32</v>
+      </c>
+      <c r="F28" s="8">
+        <v>10000</v>
+      </c>
+      <c r="G28" s="8">
+        <v>5461</v>
+      </c>
+      <c r="H28" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="8">
+        <v>8</v>
+      </c>
+      <c r="E29" s="8">
+        <v>64</v>
+      </c>
+      <c r="F29" s="8">
+        <v>18000</v>
+      </c>
+      <c r="G29" s="8">
+        <v>10923</v>
+      </c>
+      <c r="H29" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="8">
+        <v>8</v>
+      </c>
+      <c r="E30" s="8">
+        <v>64</v>
+      </c>
+      <c r="F30" s="8">
+        <v>18000</v>
+      </c>
+      <c r="G30" s="8">
+        <v>10923</v>
+      </c>
+      <c r="H30" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="8">
+        <v>16</v>
+      </c>
+      <c r="E31" s="8">
+        <v>128</v>
+      </c>
+      <c r="F31" s="8">
+        <v>28000</v>
+      </c>
+      <c r="G31" s="8">
+        <v>21845</v>
+      </c>
+      <c r="H31" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="8">
+        <v>16</v>
+      </c>
+      <c r="E32" s="8">
+        <v>128</v>
+      </c>
+      <c r="F32" s="8">
+        <v>28000</v>
+      </c>
+      <c r="G32" s="8">
+        <v>21845</v>
+      </c>
+      <c r="H32" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="8">
+        <v>20</v>
+      </c>
+      <c r="E33" s="8">
+        <v>160</v>
+      </c>
+      <c r="F33" s="8">
+        <v>28000</v>
+      </c>
+      <c r="G33" s="8">
+        <v>27306</v>
+      </c>
+      <c r="H33" s="8">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="8">
+        <v>20</v>
+      </c>
+      <c r="E34" s="8">
+        <v>160</v>
+      </c>
+      <c r="F34" s="8">
+        <v>28000</v>
+      </c>
+      <c r="G34" s="8">
+        <v>27306</v>
+      </c>
+      <c r="H34" s="8">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="8">
+        <v>32</v>
+      </c>
+      <c r="E35" s="8">
+        <v>256</v>
+      </c>
+      <c r="F35" s="8">
+        <v>38000</v>
+      </c>
+      <c r="G35" s="8">
+        <v>43691</v>
+      </c>
+      <c r="H35" s="8">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="8">
+        <v>32</v>
+      </c>
+      <c r="E36" s="8">
+        <v>256</v>
+      </c>
+      <c r="F36" s="8">
+        <v>38000</v>
+      </c>
+      <c r="G36" s="8">
+        <v>43691</v>
+      </c>
+      <c r="H36" s="8">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="8">
+        <v>48</v>
+      </c>
+      <c r="E37" s="8">
+        <v>384</v>
+      </c>
+      <c r="F37" s="8">
+        <v>48000</v>
+      </c>
+      <c r="G37" s="8">
+        <v>65536</v>
+      </c>
+      <c r="H37" s="8">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="8">
+        <v>48</v>
+      </c>
+      <c r="E38" s="8">
+        <v>384</v>
+      </c>
+      <c r="F38" s="8">
+        <v>48000</v>
+      </c>
+      <c r="G38" s="8">
+        <v>65536</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="8">
+        <v>64</v>
+      </c>
+      <c r="E39" s="8">
+        <v>504</v>
+      </c>
+      <c r="F39" s="8">
+        <v>64000</v>
+      </c>
+      <c r="G39" s="8">
+        <v>86016</v>
+      </c>
+      <c r="H39" s="8">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="8">
+        <v>64</v>
+      </c>
+      <c r="E40" s="8">
+        <v>504</v>
+      </c>
+      <c r="F40" s="8">
+        <v>64000</v>
+      </c>
+      <c r="G40" s="8">
+        <v>86016</v>
+      </c>
+      <c r="H40" s="8">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="8">
+        <v>80</v>
+      </c>
+      <c r="E41" s="8">
+        <v>504</v>
+      </c>
+      <c r="F41" s="8">
+        <v>72000</v>
+      </c>
+      <c r="G41" s="8">
+        <v>86016</v>
+      </c>
+      <c r="H41" s="8">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="8">
+        <v>2</v>
+      </c>
+      <c r="E42" s="8">
+        <v>16</v>
+      </c>
+      <c r="F42" s="8">
+        <v>5000</v>
+      </c>
+      <c r="G42" s="8">
+        <v>2731</v>
+      </c>
+      <c r="H42" s="8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="8">
+        <v>4</v>
+      </c>
+      <c r="E43" s="8">
+        <v>32</v>
+      </c>
+      <c r="F43" s="8">
+        <v>10000</v>
+      </c>
+      <c r="G43" s="8">
+        <v>5461</v>
+      </c>
+      <c r="H43" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="8">
+        <v>8</v>
+      </c>
+      <c r="E44" s="8">
+        <v>64</v>
+      </c>
+      <c r="F44" s="8">
+        <v>18000</v>
+      </c>
+      <c r="G44" s="8">
+        <v>10923</v>
+      </c>
+      <c r="H44" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="8">
+        <v>16</v>
+      </c>
+      <c r="E45" s="8">
+        <v>128</v>
+      </c>
+      <c r="F45" s="8">
+        <v>28000</v>
+      </c>
+      <c r="G45" s="8">
+        <v>21845</v>
+      </c>
+      <c r="H45" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="8">
+        <v>20</v>
+      </c>
+      <c r="E46" s="8">
+        <v>160</v>
+      </c>
+      <c r="F46" s="8">
+        <v>28000</v>
+      </c>
+      <c r="G46" s="8">
+        <v>27306</v>
+      </c>
+      <c r="H46" s="8">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="8">
+        <v>32</v>
+      </c>
+      <c r="E47" s="8">
+        <v>256</v>
+      </c>
+      <c r="F47" s="8">
+        <v>38000</v>
+      </c>
+      <c r="G47" s="8">
+        <v>43691</v>
+      </c>
+      <c r="H47" s="8">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="8">
+        <v>48</v>
+      </c>
+      <c r="E48" s="8">
+        <v>384</v>
+      </c>
+      <c r="F48" s="8">
+        <v>48000</v>
+      </c>
+      <c r="G48" s="8">
+        <v>65536</v>
+      </c>
+      <c r="H48" s="8">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="8">
+        <v>64</v>
+      </c>
+      <c r="E49" s="8">
+        <v>512</v>
+      </c>
+      <c r="F49" s="8">
+        <v>64000</v>
+      </c>
+      <c r="G49" s="8">
+        <v>87383</v>
+      </c>
+      <c r="H49" s="8">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="8">
+        <v>96</v>
+      </c>
+      <c r="E50" s="8">
+        <v>672</v>
+      </c>
+      <c r="F50" s="8">
+        <v>80000</v>
+      </c>
+      <c r="G50" s="8">
+        <v>100000</v>
+      </c>
+      <c r="H50" s="8">
+        <v>3600</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B50" xr:uid="{12D0F193-203F-4A1B-8197-1D6CABED875D}">
+      <formula1>"Burstable,GeneralPurpose,MemoryOptimized"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>